<commit_message>
updating plots to incorporate Courtney's suggestions
</commit_message>
<xml_diff>
--- a/outputs/summary_pct_pop_guild_carbon_16Sep2023_RAN.xlsx
+++ b/outputs/summary_pct_pop_guild_carbon_16Sep2023_RAN.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raenb\Documents\GitHub\es_birds_usa\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{250432A6-92A8-4644-A97F-3719153EFF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CC3493-4BC4-4611-9ECA-02ABDFBC217F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary_pct_pop_guild_carbon_16" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>more75</t>
   </si>
@@ -52,16 +65,13 @@
     <t>generalist</t>
   </si>
   <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>count</t>
+    <t># species</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -899,11 +909,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,7 +938,7 @@
         <v>0</v>
       </c>
       <c r="G1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
@@ -956,6 +966,9 @@
       <c r="E2" s="1">
         <v>0.157894736842105</v>
       </c>
+      <c r="G2">
+        <v>57</v>
+      </c>
       <c r="H2">
         <f>C2*B2</f>
         <v>25.999999999999943</v>
@@ -985,6 +998,9 @@
       <c r="E3" s="1">
         <v>0.27227722772277202</v>
       </c>
+      <c r="G3">
+        <v>202</v>
+      </c>
       <c r="H3">
         <f t="shared" ref="H3:H7" si="0">C3*B3</f>
         <v>179.99999999999997</v>
@@ -1014,6 +1030,9 @@
       <c r="E4" s="1">
         <v>0</v>
       </c>
+      <c r="G4">
+        <v>31</v>
+      </c>
       <c r="H4">
         <f t="shared" si="0"/>
         <v>11.999999999999988</v>
@@ -1043,6 +1062,9 @@
       <c r="E5" s="1">
         <v>1.6129032258064498E-2</v>
       </c>
+      <c r="G5">
+        <v>62</v>
+      </c>
       <c r="H5">
         <f t="shared" si="0"/>
         <v>7.9999999999999911</v>
@@ -1072,6 +1094,9 @@
       <c r="E6" s="1">
         <v>1.3793103448275799E-2</v>
       </c>
+      <c r="G6">
+        <v>146</v>
+      </c>
       <c r="H6" s="2">
         <f>C6*B6</f>
         <v>60.413793103448157</v>
@@ -1100,6 +1125,9 @@
       </c>
       <c r="E7" s="1">
         <v>0</v>
+      </c>
+      <c r="G7">
+        <v>38</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>

</xml_diff>